<commit_message>
freeze rows and columns. resort by total points. rename attachment
</commit_message>
<xml_diff>
--- a/data/weekly_update/2017/2017_week_1_standings.xlsx
+++ b/data/weekly_update/2017/2017_week_1_standings.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="83">
   <si>
     <t>Rank</t>
   </si>
@@ -254,6 +254,18 @@
   </si>
   <si>
     <t>NYG</t>
+  </si>
+  <si>
+    <t>T.Morstead</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>R.Quigley</t>
+  </si>
+  <si>
+    <t>MIN</t>
   </si>
 </sst>
 </file>
@@ -616,8 +628,10 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -690,11 +704,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2525,6 +2541,136 @@
         <v>0</v>
       </c>
     </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="3">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="4">
+        <v>2</v>
+      </c>
+      <c r="F29" s="4">
+        <v>125</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0</v>
+      </c>
+      <c r="K29" s="4">
+        <v>2</v>
+      </c>
+      <c r="L29" s="4">
+        <v>1</v>
+      </c>
+      <c r="M29" s="4">
+        <v>0</v>
+      </c>
+      <c r="N29" s="4">
+        <v>1</v>
+      </c>
+      <c r="O29" s="4">
+        <v>1</v>
+      </c>
+      <c r="P29" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>0</v>
+      </c>
+      <c r="R29" s="4">
+        <v>1</v>
+      </c>
+      <c r="S29" s="4">
+        <v>13</v>
+      </c>
+      <c r="T29" s="4">
+        <v>2</v>
+      </c>
+      <c r="U29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30" s="3">
+        <v>1</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="4">
+        <v>1</v>
+      </c>
+      <c r="F30" s="4">
+        <v>52</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0</v>
+      </c>
+      <c r="I30" s="4">
+        <v>0</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0</v>
+      </c>
+      <c r="K30" s="4">
+        <v>1</v>
+      </c>
+      <c r="L30" s="4">
+        <v>0</v>
+      </c>
+      <c r="M30" s="4">
+        <v>0</v>
+      </c>
+      <c r="N30" s="4">
+        <v>0</v>
+      </c>
+      <c r="O30" s="4">
+        <v>0</v>
+      </c>
+      <c r="P30" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>0</v>
+      </c>
+      <c r="R30" s="4">
+        <v>1</v>
+      </c>
+      <c r="S30" s="4">
+        <v>0</v>
+      </c>
+      <c r="T30" s="4">
+        <v>2</v>
+      </c>
+      <c r="U30" s="4">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2532,11 +2678,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3964,16 +4112,16 @@
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="3" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C25" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D25" s="3">
-        <v>302</v>
+        <v>52</v>
       </c>
       <c r="E25" s="4">
         <v>0</v>
@@ -3985,10 +4133,10 @@
         <v>0</v>
       </c>
       <c r="H25" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I25" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J25" s="4">
         <v>0</v>
@@ -3997,7 +4145,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M25" s="4">
         <v>0</v>
@@ -4009,30 +4157,30 @@
         <v>0</v>
       </c>
       <c r="P25" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q25" s="4">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="R25" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S25" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:19">
       <c r="A26" s="3" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="C26" s="3">
         <v>6</v>
       </c>
       <c r="D26" s="3">
-        <v>250</v>
+        <v>302</v>
       </c>
       <c r="E26" s="4">
         <v>0</v>
@@ -4041,13 +4189,13 @@
         <v>0</v>
       </c>
       <c r="G26" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H26" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I26" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J26" s="4">
         <v>0</v>
@@ -4059,7 +4207,7 @@
         <v>2</v>
       </c>
       <c r="M26" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N26" s="4">
         <v>0</v>
@@ -4071,27 +4219,27 @@
         <v>3</v>
       </c>
       <c r="Q26" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R26" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S26" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:19">
       <c r="A27" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C27" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D27" s="3">
-        <v>216</v>
+        <v>250</v>
       </c>
       <c r="E27" s="4">
         <v>0</v>
@@ -4100,13 +4248,13 @@
         <v>0</v>
       </c>
       <c r="G27" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H27" s="4">
         <v>1</v>
       </c>
       <c r="I27" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J27" s="4">
         <v>0</v>
@@ -4118,7 +4266,7 @@
         <v>2</v>
       </c>
       <c r="M27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N27" s="4">
         <v>0</v>
@@ -4127,13 +4275,13 @@
         <v>0</v>
       </c>
       <c r="P27" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q27" s="4">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="R27" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S27" s="4">
         <v>0</v>
@@ -4141,60 +4289,178 @@
     </row>
     <row r="28" spans="1:19">
       <c r="A28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="3">
+        <v>5</v>
+      </c>
+      <c r="D28" s="3">
+        <v>216</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0</v>
+      </c>
+      <c r="G28" s="4">
+        <v>3</v>
+      </c>
+      <c r="H28" s="4">
+        <v>1</v>
+      </c>
+      <c r="I28" s="4">
+        <v>2</v>
+      </c>
+      <c r="J28" s="4">
+        <v>0</v>
+      </c>
+      <c r="K28" s="4">
+        <v>0</v>
+      </c>
+      <c r="L28" s="4">
+        <v>2</v>
+      </c>
+      <c r="M28" s="4">
+        <v>0</v>
+      </c>
+      <c r="N28" s="4">
+        <v>0</v>
+      </c>
+      <c r="O28" s="4">
+        <v>0</v>
+      </c>
+      <c r="P28" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>7</v>
+      </c>
+      <c r="R28" s="4">
+        <v>1</v>
+      </c>
+      <c r="S28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2</v>
+      </c>
+      <c r="D29" s="3">
+        <v>125</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+      <c r="I29" s="4">
+        <v>2</v>
+      </c>
+      <c r="J29" s="4">
+        <v>1</v>
+      </c>
+      <c r="K29" s="4">
+        <v>0</v>
+      </c>
+      <c r="L29" s="4">
+        <v>1</v>
+      </c>
+      <c r="M29" s="4">
+        <v>1</v>
+      </c>
+      <c r="N29" s="4">
+        <v>0</v>
+      </c>
+      <c r="O29" s="4">
+        <v>0</v>
+      </c>
+      <c r="P29" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>13</v>
+      </c>
+      <c r="R29" s="4">
+        <v>2</v>
+      </c>
+      <c r="S29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C30" s="3">
         <v>4</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D30" s="3">
         <v>162</v>
       </c>
-      <c r="E28" s="4">
-        <v>0</v>
-      </c>
-      <c r="F28" s="4">
-        <v>0</v>
-      </c>
-      <c r="G28" s="4">
-        <v>2</v>
-      </c>
-      <c r="H28" s="4">
-        <v>1</v>
-      </c>
-      <c r="I28" s="4">
-        <v>1</v>
-      </c>
-      <c r="J28" s="4">
-        <v>0</v>
-      </c>
-      <c r="K28" s="4">
-        <v>0</v>
-      </c>
-      <c r="L28" s="4">
-        <v>2</v>
-      </c>
-      <c r="M28" s="4">
-        <v>1</v>
-      </c>
-      <c r="N28" s="4">
-        <v>0</v>
-      </c>
-      <c r="O28" s="4">
-        <v>0</v>
-      </c>
-      <c r="P28" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="4">
-        <v>0</v>
-      </c>
-      <c r="R28" s="4">
-        <v>2</v>
-      </c>
-      <c r="S28" s="4">
+      <c r="E30" s="4">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4">
+        <v>2</v>
+      </c>
+      <c r="H30" s="4">
+        <v>1</v>
+      </c>
+      <c r="I30" s="4">
+        <v>1</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0</v>
+      </c>
+      <c r="K30" s="4">
+        <v>0</v>
+      </c>
+      <c r="L30" s="4">
+        <v>2</v>
+      </c>
+      <c r="M30" s="4">
+        <v>1</v>
+      </c>
+      <c r="N30" s="4">
+        <v>0</v>
+      </c>
+      <c r="O30" s="4">
+        <v>0</v>
+      </c>
+      <c r="P30" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>0</v>
+      </c>
+      <c r="R30" s="4">
+        <v>2</v>
+      </c>
+      <c r="S30" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4205,11 +4471,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T28"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4290,10 +4558,10 @@
         <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
@@ -4302,13 +4570,13 @@
         <v>0</v>
       </c>
       <c r="G2" s="5">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="H2" s="5">
         <v>0</v>
       </c>
       <c r="I2" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J2" s="5">
         <v>0</v>
@@ -4317,31 +4585,31 @@
         <v>0</v>
       </c>
       <c r="L2" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M2" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N2" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O2" s="5">
         <v>0</v>
       </c>
       <c r="P2" s="5">
-        <v>-0.1333333333333336</v>
+        <v>0.08333333333333358</v>
       </c>
       <c r="Q2" s="5">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="R2" s="5">
-        <v>0.6000000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="S2" s="5">
         <v>-0</v>
       </c>
       <c r="T2" s="5">
-        <v>5.366666666666667</v>
+        <v>8.733333333333334</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -4352,10 +4620,10 @@
         <v>25</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
@@ -4364,46 +4632,46 @@
         <v>0.4</v>
       </c>
       <c r="G3" s="5">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H3" s="5">
         <v>0</v>
       </c>
       <c r="I3" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J3" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K3" s="5">
         <v>0</v>
       </c>
       <c r="L3" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M3" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="N3" s="5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O3" s="5">
         <v>0</v>
       </c>
       <c r="P3" s="5">
-        <v>0.7666666666666665</v>
+        <v>0.3799999999999997</v>
       </c>
       <c r="Q3" s="5">
-        <v>-0.4</v>
+        <v>0.3</v>
       </c>
       <c r="R3" s="5">
-        <v>0.6000000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="S3" s="5">
         <v>-0</v>
       </c>
       <c r="T3" s="5">
-        <v>5.616666666666667</v>
+        <v>8.380000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -4414,10 +4682,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="E4" s="5">
         <v>0</v>
@@ -4432,7 +4700,7 @@
         <v>0.15</v>
       </c>
       <c r="I4" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J4" s="5">
         <v>0</v>
@@ -4441,31 +4709,31 @@
         <v>0</v>
       </c>
       <c r="L4" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M4" s="5">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="N4" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O4" s="5">
         <v>0</v>
       </c>
       <c r="P4" s="5">
-        <v>-0.1399999999999999</v>
+        <v>0.45</v>
       </c>
       <c r="Q4" s="5">
-        <v>-0.9</v>
+        <v>-0.025</v>
       </c>
       <c r="R4" s="5">
-        <v>0.6000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="S4" s="5">
         <v>-0</v>
       </c>
       <c r="T4" s="5">
-        <v>6.210000000000001</v>
+        <v>8.025</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -4476,10 +4744,10 @@
         <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -4491,22 +4759,22 @@
         <v>0</v>
       </c>
       <c r="H5" s="5">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="I5" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K5" s="5">
         <v>0</v>
       </c>
       <c r="L5" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M5" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N5" s="5">
         <v>0</v>
@@ -4515,19 +4783,19 @@
         <v>0</v>
       </c>
       <c r="P5" s="5">
-        <v>-0.4666666666666665</v>
+        <v>1.75</v>
       </c>
       <c r="Q5" s="5">
-        <v>-0.65</v>
+        <v>0.4</v>
       </c>
       <c r="R5" s="5">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="S5" s="5">
         <v>-0</v>
       </c>
       <c r="T5" s="5">
-        <v>2.683333333333334</v>
+        <v>6.850000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -4538,10 +4806,10 @@
         <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
@@ -4550,25 +4818,25 @@
         <v>0</v>
       </c>
       <c r="G6" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H6" s="5">
         <v>0</v>
       </c>
       <c r="I6" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J6" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="K6" s="5">
         <v>0</v>
       </c>
       <c r="L6" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M6" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N6" s="5">
         <v>0</v>
@@ -4577,10 +4845,10 @@
         <v>0</v>
       </c>
       <c r="P6" s="5">
-        <v>1.433333333333334</v>
+        <v>-1.025</v>
       </c>
       <c r="Q6" s="5">
-        <v>0.6000000000000001</v>
+        <v>-0.1</v>
       </c>
       <c r="R6" s="5">
         <v>0.5</v>
@@ -4589,7 +4857,7 @@
         <v>-0</v>
       </c>
       <c r="T6" s="5">
-        <v>6.283333333333333</v>
+        <v>6.625</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -4600,10 +4868,10 @@
         <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
@@ -4612,22 +4880,22 @@
         <v>0</v>
       </c>
       <c r="G7" s="5">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="H7" s="5">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I7" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J7" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K7" s="5">
         <v>0</v>
       </c>
       <c r="L7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="5">
         <v>0</v>
@@ -4639,10 +4907,10 @@
         <v>0</v>
       </c>
       <c r="P7" s="5">
-        <v>0.6666666666666665</v>
+        <v>1.433333333333334</v>
       </c>
       <c r="Q7" s="5">
-        <v>0</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="R7" s="5">
         <v>0.5</v>
@@ -4651,7 +4919,7 @@
         <v>-0</v>
       </c>
       <c r="T7" s="5">
-        <v>4.566666666666666</v>
+        <v>6.283333333333333</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -4662,10 +4930,10 @@
         <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
@@ -4674,13 +4942,13 @@
         <v>0</v>
       </c>
       <c r="G8" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="H8" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="5">
         <v>0</v>
@@ -4689,7 +4957,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M8" s="5">
         <v>1.5</v>
@@ -4701,19 +4969,19 @@
         <v>0</v>
       </c>
       <c r="P8" s="5">
-        <v>-1.025</v>
+        <v>-0.1399999999999999</v>
       </c>
       <c r="Q8" s="5">
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="R8" s="5">
-        <v>0.5</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="S8" s="5">
         <v>-0</v>
       </c>
       <c r="T8" s="5">
-        <v>6.625</v>
+        <v>6.210000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -4724,34 +4992,34 @@
         <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E9" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F9" s="5">
         <v>0</v>
       </c>
       <c r="G9" s="5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H9" s="5">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I9" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J9" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K9" s="5">
         <v>0</v>
       </c>
       <c r="L9" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M9" s="5">
         <v>0.75</v>
@@ -4763,19 +5031,19 @@
         <v>0</v>
       </c>
       <c r="P9" s="5">
-        <v>-0.3333333333333336</v>
+        <v>0.3399999999999999</v>
       </c>
       <c r="Q9" s="5">
-        <v>-0.4333333333333333</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="R9" s="5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="S9" s="5">
         <v>-0</v>
       </c>
       <c r="T9" s="5">
-        <v>4.033333333333333</v>
+        <v>6.206666666666667</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -4786,10 +5054,10 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
@@ -4798,46 +5066,46 @@
         <v>0.4</v>
       </c>
       <c r="G10" s="5">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="H10" s="5">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I10" s="5">
         <v>2</v>
       </c>
       <c r="J10" s="5">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5">
+        <v>1</v>
+      </c>
+      <c r="M10" s="5">
         <v>0.75</v>
       </c>
-      <c r="K10" s="5">
-        <v>0</v>
-      </c>
-      <c r="L10" s="5">
-        <v>0</v>
-      </c>
-      <c r="M10" s="5">
-        <v>0</v>
-      </c>
       <c r="N10" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O10" s="5">
         <v>0</v>
       </c>
       <c r="P10" s="5">
-        <v>0.175</v>
+        <v>0.7666666666666665</v>
       </c>
       <c r="Q10" s="5">
-        <v>1.2</v>
+        <v>-0.4</v>
       </c>
       <c r="R10" s="5">
-        <v>0.4</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="S10" s="5">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="T10" s="5">
-        <v>4.325</v>
+        <v>5.616666666666667</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -4848,22 +5116,22 @@
         <v>25</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="E11" s="5">
         <v>0</v>
       </c>
       <c r="F11" s="5">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G11" s="5">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H11" s="5">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I11" s="5">
         <v>1</v>
@@ -4875,7 +5143,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M11" s="5">
         <v>0</v>
@@ -4887,19 +5155,19 @@
         <v>0</v>
       </c>
       <c r="P11" s="5">
-        <v>0.2</v>
+        <v>-0.1333333333333336</v>
       </c>
       <c r="Q11" s="5">
-        <v>-0.4</v>
+        <v>-0.1</v>
       </c>
       <c r="R11" s="5">
-        <v>0.4</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="S11" s="5">
-        <v>-0.5</v>
+        <v>-0</v>
       </c>
       <c r="T11" s="5">
-        <v>3.5</v>
+        <v>5.366666666666667</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -4910,10 +5178,10 @@
         <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
@@ -4922,13 +5190,13 @@
         <v>0</v>
       </c>
       <c r="G12" s="5">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="H12" s="5">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="I12" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J12" s="5">
         <v>0</v>
@@ -4937,31 +5205,31 @@
         <v>0</v>
       </c>
       <c r="L12" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="N12" s="5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O12" s="5">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="P12" s="5">
-        <v>-0.25</v>
+        <v>0.5333333333333335</v>
       </c>
       <c r="Q12" s="5">
-        <v>-0.75</v>
+        <v>-0.4</v>
       </c>
       <c r="R12" s="5">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="S12" s="5">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="T12" s="5">
-        <v>2.65</v>
+        <v>4.683333333333333</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -4972,22 +5240,22 @@
         <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="E13" s="5">
         <v>0</v>
       </c>
       <c r="F13" s="5">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G13" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="H13" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I13" s="5">
         <v>2</v>
@@ -4999,7 +5267,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M13" s="5">
         <v>0</v>
@@ -5011,19 +5279,19 @@
         <v>0</v>
       </c>
       <c r="P13" s="5">
-        <v>-0.2166666666666665</v>
+        <v>-0.1799999999999997</v>
       </c>
       <c r="Q13" s="5">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="R13" s="5">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="S13" s="5">
-        <v>-0.5</v>
+        <v>-0</v>
       </c>
       <c r="T13" s="5">
-        <v>3.483333333333333</v>
+        <v>4.62</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -5034,34 +5302,34 @@
         <v>25</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="E14" s="5">
         <v>0</v>
       </c>
       <c r="F14" s="5">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G14" s="5">
         <v>0.25</v>
       </c>
       <c r="H14" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I14" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J14" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="K14" s="5">
         <v>0</v>
       </c>
       <c r="L14" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M14" s="5">
         <v>0</v>
@@ -5073,19 +5341,19 @@
         <v>0</v>
       </c>
       <c r="P14" s="5">
-        <v>0.3799999999999997</v>
+        <v>0.6666666666666665</v>
       </c>
       <c r="Q14" s="5">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="R14" s="5">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="S14" s="5">
         <v>-0</v>
       </c>
       <c r="T14" s="5">
-        <v>8.380000000000001</v>
+        <v>4.566666666666666</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -5096,58 +5364,58 @@
         <v>25</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E15" s="5">
         <v>0</v>
       </c>
       <c r="F15" s="5">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G15" s="5">
         <v>0.25</v>
       </c>
       <c r="H15" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I15" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J15" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K15" s="5">
         <v>0</v>
       </c>
       <c r="L15" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M15" s="5">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="N15" s="5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O15" s="5">
         <v>0</v>
       </c>
       <c r="P15" s="5">
-        <v>0.08333333333333358</v>
+        <v>0.175</v>
       </c>
       <c r="Q15" s="5">
-        <v>-0.9</v>
+        <v>1.2</v>
       </c>
       <c r="R15" s="5">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="S15" s="5">
-        <v>-0</v>
+        <v>-1</v>
       </c>
       <c r="T15" s="5">
-        <v>8.733333333333334</v>
+        <v>4.325</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -5158,10 +5426,10 @@
         <v>25</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E16" s="5">
         <v>0</v>
@@ -5170,10 +5438,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H16" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I16" s="5">
         <v>1</v>
@@ -5185,10 +5453,10 @@
         <v>0</v>
       </c>
       <c r="L16" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M16" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N16" s="5">
         <v>0</v>
@@ -5197,19 +5465,19 @@
         <v>0</v>
       </c>
       <c r="P16" s="5">
-        <v>-0.1200000000000003</v>
+        <v>-0.45</v>
       </c>
       <c r="Q16" s="5">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="R16" s="5">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="S16" s="5">
         <v>-0</v>
       </c>
       <c r="T16" s="5">
-        <v>2.98</v>
+        <v>4.15</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -5220,10 +5488,10 @@
         <v>25</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
@@ -5232,13 +5500,13 @@
         <v>0</v>
       </c>
       <c r="G17" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H17" s="5">
         <v>0.15</v>
       </c>
       <c r="I17" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J17" s="5">
         <v>0</v>
@@ -5253,25 +5521,25 @@
         <v>0.75</v>
       </c>
       <c r="N17" s="5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O17" s="5">
         <v>0</v>
       </c>
       <c r="P17" s="5">
-        <v>0.45</v>
+        <v>-0.3333333333333336</v>
       </c>
       <c r="Q17" s="5">
-        <v>-0.025</v>
+        <v>-0.4333333333333333</v>
       </c>
       <c r="R17" s="5">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="S17" s="5">
         <v>-0</v>
       </c>
       <c r="T17" s="5">
-        <v>8.025</v>
+        <v>4.033333333333333</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -5282,34 +5550,34 @@
         <v>25</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E18" s="5">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F18" s="5">
         <v>0</v>
       </c>
       <c r="G18" s="5">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H18" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I18" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J18" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="K18" s="5">
         <v>0</v>
       </c>
       <c r="L18" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M18" s="5">
         <v>0.75</v>
@@ -5321,19 +5589,19 @@
         <v>0</v>
       </c>
       <c r="P18" s="5">
-        <v>0.3399999999999999</v>
+        <v>-0.2600000000000002</v>
       </c>
       <c r="Q18" s="5">
-        <v>0.1666666666666666</v>
+        <v>-0.1333333333333333</v>
       </c>
       <c r="R18" s="5">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="S18" s="5">
         <v>-0</v>
       </c>
       <c r="T18" s="5">
-        <v>6.206666666666667</v>
+        <v>3.756666666666667</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -5344,22 +5612,22 @@
         <v>25</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="E19" s="5">
         <v>0</v>
       </c>
       <c r="F19" s="5">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G19" s="5">
         <v>0.25</v>
       </c>
       <c r="H19" s="5">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="I19" s="5">
         <v>1</v>
@@ -5371,7 +5639,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M19" s="5">
         <v>0</v>
@@ -5383,19 +5651,19 @@
         <v>0</v>
       </c>
       <c r="P19" s="5">
-        <v>0.08333333333333358</v>
+        <v>0.2</v>
       </c>
       <c r="Q19" s="5">
-        <v>0.2333333333333334</v>
+        <v>-0.4</v>
       </c>
       <c r="R19" s="5">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="S19" s="5">
-        <v>-0</v>
+        <v>-0.5</v>
       </c>
       <c r="T19" s="5">
-        <v>2.066666666666667</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -5406,25 +5674,25 @@
         <v>25</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="E20" s="5">
         <v>0</v>
       </c>
       <c r="F20" s="5">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G20" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H20" s="5">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I20" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J20" s="5">
         <v>0</v>
@@ -5433,7 +5701,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" s="5">
         <v>0</v>
@@ -5445,19 +5713,19 @@
         <v>0</v>
       </c>
       <c r="P20" s="5">
-        <v>0.1</v>
+        <v>-0.2166666666666665</v>
       </c>
       <c r="Q20" s="5">
-        <v>0.7000000000000001</v>
+        <v>0</v>
       </c>
       <c r="R20" s="5">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="S20" s="5">
         <v>-0.5</v>
       </c>
       <c r="T20" s="5">
-        <v>1.65</v>
+        <v>3.483333333333333</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -5468,10 +5736,10 @@
         <v>25</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="E21" s="5">
         <v>0</v>
@@ -5480,13 +5748,13 @@
         <v>0</v>
       </c>
       <c r="G21" s="5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H21" s="5">
         <v>0</v>
       </c>
       <c r="I21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="5">
         <v>0</v>
@@ -5498,7 +5766,7 @@
         <v>1</v>
       </c>
       <c r="M21" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="N21" s="5">
         <v>0</v>
@@ -5507,19 +5775,19 @@
         <v>0</v>
       </c>
       <c r="P21" s="5">
-        <v>-1.025</v>
+        <v>-0.1200000000000003</v>
       </c>
       <c r="Q21" s="5">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="R21" s="5">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="S21" s="5">
         <v>-0</v>
       </c>
       <c r="T21" s="5">
-        <v>1.425</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -5530,10 +5798,10 @@
         <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="E22" s="5">
         <v>0</v>
@@ -5542,46 +5810,46 @@
         <v>0</v>
       </c>
       <c r="G22" s="5">
+        <v>0</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="I22" s="5">
+        <v>1</v>
+      </c>
+      <c r="J22" s="5">
+        <v>0</v>
+      </c>
+      <c r="K22" s="5">
+        <v>0</v>
+      </c>
+      <c r="L22" s="5">
+        <v>2</v>
+      </c>
+      <c r="M22" s="5">
+        <v>0</v>
+      </c>
+      <c r="N22" s="5">
+        <v>0</v>
+      </c>
+      <c r="O22" s="5">
+        <v>0</v>
+      </c>
+      <c r="P22" s="5">
+        <v>-0.4666666666666665</v>
+      </c>
+      <c r="Q22" s="5">
+        <v>-0.65</v>
+      </c>
+      <c r="R22" s="5">
         <v>0.5</v>
-      </c>
-      <c r="H22" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="I22" s="5">
-        <v>1</v>
-      </c>
-      <c r="J22" s="5">
-        <v>0</v>
-      </c>
-      <c r="K22" s="5">
-        <v>0</v>
-      </c>
-      <c r="L22" s="5">
-        <v>2</v>
-      </c>
-      <c r="M22" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="N22" s="5">
-        <v>0</v>
-      </c>
-      <c r="O22" s="5">
-        <v>0</v>
-      </c>
-      <c r="P22" s="5">
-        <v>-0.45</v>
-      </c>
-      <c r="Q22" s="5">
-        <v>0</v>
-      </c>
-      <c r="R22" s="5">
-        <v>0.2</v>
       </c>
       <c r="S22" s="5">
         <v>-0</v>
       </c>
       <c r="T22" s="5">
-        <v>4.15</v>
+        <v>2.683333333333334</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -5592,10 +5860,10 @@
         <v>25</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E23" s="5">
         <v>0</v>
@@ -5604,46 +5872,46 @@
         <v>0</v>
       </c>
       <c r="G23" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0</v>
+      </c>
+      <c r="I23" s="5">
+        <v>1</v>
+      </c>
+      <c r="J23" s="5">
+        <v>0</v>
+      </c>
+      <c r="K23" s="5">
+        <v>0</v>
+      </c>
+      <c r="L23" s="5">
+        <v>1</v>
+      </c>
+      <c r="M23" s="5">
         <v>0.75</v>
       </c>
-      <c r="H23" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="I23" s="5">
-        <v>2</v>
-      </c>
-      <c r="J23" s="5">
-        <v>0</v>
-      </c>
-      <c r="K23" s="5">
-        <v>0</v>
-      </c>
-      <c r="L23" s="5">
-        <v>2</v>
-      </c>
-      <c r="M23" s="5">
-        <v>0</v>
-      </c>
       <c r="N23" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O23" s="5">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="P23" s="5">
-        <v>-0.1799999999999997</v>
+        <v>-0.25</v>
       </c>
       <c r="Q23" s="5">
-        <v>-0.2</v>
+        <v>-0.75</v>
       </c>
       <c r="R23" s="5">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="S23" s="5">
-        <v>-0</v>
+        <v>-0.5</v>
       </c>
       <c r="T23" s="5">
-        <v>4.62</v>
+        <v>2.65</v>
       </c>
     </row>
     <row r="24" spans="1:20">
@@ -5654,10 +5922,10 @@
         <v>25</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="E24" s="5">
         <v>0</v>
@@ -5666,13 +5934,13 @@
         <v>0</v>
       </c>
       <c r="G24" s="5">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H24" s="5">
-        <v>0.45</v>
+        <v>0.3</v>
       </c>
       <c r="I24" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J24" s="5">
         <v>0</v>
@@ -5681,7 +5949,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M24" s="5">
         <v>0</v>
@@ -5693,19 +5961,19 @@
         <v>0</v>
       </c>
       <c r="P24" s="5">
-        <v>0.5333333333333335</v>
+        <v>0.08333333333333358</v>
       </c>
       <c r="Q24" s="5">
-        <v>-0.4</v>
+        <v>0.2333333333333334</v>
       </c>
       <c r="R24" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="S24" s="5">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="T24" s="5">
-        <v>4.683333333333333</v>
+        <v>2.066666666666667</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -5716,10 +5984,10 @@
         <v>25</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="E25" s="5">
         <v>0</v>
@@ -5728,13 +5996,13 @@
         <v>0</v>
       </c>
       <c r="G25" s="5">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="H25" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="5">
         <v>0</v>
@@ -5743,7 +6011,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" s="5">
         <v>0</v>
@@ -5755,19 +6023,19 @@
         <v>0</v>
       </c>
       <c r="P25" s="5">
-        <v>-0.425</v>
+        <v>0.1</v>
       </c>
       <c r="Q25" s="5">
-        <v>-0.6666666666666666</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="R25" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="S25" s="5">
-        <v>-0</v>
+        <v>-0.5</v>
       </c>
       <c r="T25" s="5">
-        <v>0.2583333333333333</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="26" spans="1:20">
@@ -5778,25 +6046,25 @@
         <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="E26" s="5">
         <v>0</v>
       </c>
       <c r="F26" s="5">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G26" s="5">
         <v>0.5</v>
       </c>
       <c r="H26" s="5">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I26" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" s="5">
         <v>0</v>
@@ -5805,10 +6073,10 @@
         <v>0</v>
       </c>
       <c r="L26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N26" s="5">
         <v>0</v>
@@ -5817,19 +6085,19 @@
         <v>0</v>
       </c>
       <c r="P26" s="5">
-        <v>-0.01666666666666643</v>
+        <v>-1.025</v>
       </c>
       <c r="Q26" s="5">
-        <v>-0.9</v>
+        <v>0</v>
       </c>
       <c r="R26" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="S26" s="5">
         <v>-0</v>
       </c>
       <c r="T26" s="5">
-        <v>1.233333333333333</v>
+        <v>1.425</v>
       </c>
     </row>
     <row r="27" spans="1:20">
@@ -5840,25 +6108,25 @@
         <v>25</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="E27" s="5">
         <v>0</v>
       </c>
       <c r="F27" s="5">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G27" s="5">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H27" s="5">
         <v>0.15</v>
       </c>
       <c r="I27" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J27" s="5">
         <v>0</v>
@@ -5867,10 +6135,10 @@
         <v>0</v>
       </c>
       <c r="L27" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="N27" s="5">
         <v>0</v>
@@ -5879,19 +6147,19 @@
         <v>0</v>
       </c>
       <c r="P27" s="5">
-        <v>-0.2600000000000002</v>
+        <v>-0.01666666666666643</v>
       </c>
       <c r="Q27" s="5">
-        <v>-0.1333333333333333</v>
+        <v>-0.9</v>
       </c>
       <c r="R27" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="S27" s="5">
         <v>-0</v>
       </c>
       <c r="T27" s="5">
-        <v>3.756666666666667</v>
+        <v>1.233333333333333</v>
       </c>
     </row>
     <row r="28" spans="1:20">
@@ -5902,10 +6170,10 @@
         <v>25</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="E28" s="5">
         <v>0</v>
@@ -5941,19 +6209,143 @@
         <v>0</v>
       </c>
       <c r="P28" s="5">
-        <v>0.5</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="Q28" s="5">
         <v>-0.9</v>
       </c>
       <c r="R28" s="5">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S28" s="5">
         <v>-0</v>
       </c>
       <c r="T28" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
+        <v>1</v>
+      </c>
+      <c r="J29" s="5">
+        <v>0</v>
+      </c>
+      <c r="K29" s="5">
+        <v>0</v>
+      </c>
+      <c r="L29" s="5">
+        <v>0</v>
+      </c>
+      <c r="M29" s="5">
+        <v>0</v>
+      </c>
+      <c r="N29" s="5">
+        <v>0</v>
+      </c>
+      <c r="O29" s="5">
+        <v>0</v>
+      </c>
+      <c r="P29" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="Q29" s="5">
+        <v>-0.9</v>
+      </c>
+      <c r="R29" s="5">
+        <v>0</v>
+      </c>
+      <c r="S29" s="5">
+        <v>-0</v>
+      </c>
+      <c r="T29" s="5">
         <v>0.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
+        <v>0</v>
+      </c>
+      <c r="J30" s="5">
+        <v>0</v>
+      </c>
+      <c r="K30" s="5">
+        <v>0</v>
+      </c>
+      <c r="L30" s="5">
+        <v>1</v>
+      </c>
+      <c r="M30" s="5">
+        <v>0</v>
+      </c>
+      <c r="N30" s="5">
+        <v>0</v>
+      </c>
+      <c r="O30" s="5">
+        <v>0</v>
+      </c>
+      <c r="P30" s="5">
+        <v>-0.425</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>-0.6666666666666666</v>
+      </c>
+      <c r="R30" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="S30" s="5">
+        <v>-0</v>
+      </c>
+      <c r="T30" s="5">
+        <v>0.2583333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add to distro. week 2 TNF update
</commit_message>
<xml_diff>
--- a/data/weekly_update/2017/2017_week_1_standings.xlsx
+++ b/data/weekly_update/2017/2017_week_1_standings.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="87">
   <si>
     <t>Rank</t>
   </si>
@@ -266,6 +266,18 @@
   </si>
   <si>
     <t>MIN</t>
+  </si>
+  <si>
+    <t>R.Dixon</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>D.Kaser</t>
+  </si>
+  <si>
+    <t>LAC</t>
   </si>
 </sst>
 </file>
@@ -704,7 +716,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U30"/>
+  <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -2555,10 +2567,10 @@
         <v>80</v>
       </c>
       <c r="E29" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F29" s="4">
-        <v>125</v>
+        <v>171</v>
       </c>
       <c r="G29" s="4">
         <v>0</v>
@@ -2594,13 +2606,13 @@
         <v>0</v>
       </c>
       <c r="R29" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S29" s="4">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="T29" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="U29" s="4">
         <v>0</v>
@@ -2620,10 +2632,10 @@
         <v>82</v>
       </c>
       <c r="E30" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F30" s="4">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="G30" s="4">
         <v>0</v>
@@ -2632,7 +2644,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="4">
         <v>0</v>
@@ -2647,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="N30" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O30" s="4">
         <v>0</v>
@@ -2665,9 +2677,139 @@
         <v>0</v>
       </c>
       <c r="T30" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="U30" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31" s="3">
+        <v>1</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="4">
+        <v>3</v>
+      </c>
+      <c r="F31" s="4">
+        <v>144</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0</v>
+      </c>
+      <c r="I31" s="4">
+        <v>2</v>
+      </c>
+      <c r="J31" s="4">
+        <v>0</v>
+      </c>
+      <c r="K31" s="4">
+        <v>2</v>
+      </c>
+      <c r="L31" s="4">
+        <v>0</v>
+      </c>
+      <c r="M31" s="4">
+        <v>0</v>
+      </c>
+      <c r="N31" s="4">
+        <v>2</v>
+      </c>
+      <c r="O31" s="4">
+        <v>0</v>
+      </c>
+      <c r="P31" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>0</v>
+      </c>
+      <c r="R31" s="4">
+        <v>1</v>
+      </c>
+      <c r="S31" s="4">
+        <v>-3</v>
+      </c>
+      <c r="T31" s="4">
+        <v>4</v>
+      </c>
+      <c r="U31" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" s="3">
+        <v>1</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" s="4">
+        <v>5</v>
+      </c>
+      <c r="F32" s="4">
+        <v>230</v>
+      </c>
+      <c r="G32" s="4">
+        <v>0</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0</v>
+      </c>
+      <c r="I32" s="4">
+        <v>0</v>
+      </c>
+      <c r="J32" s="4">
+        <v>1</v>
+      </c>
+      <c r="K32" s="4">
+        <v>2</v>
+      </c>
+      <c r="L32" s="4">
+        <v>1</v>
+      </c>
+      <c r="M32" s="4">
+        <v>0</v>
+      </c>
+      <c r="N32" s="4">
+        <v>2</v>
+      </c>
+      <c r="O32" s="4">
+        <v>0</v>
+      </c>
+      <c r="P32" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>0</v>
+      </c>
+      <c r="R32" s="4">
+        <v>3</v>
+      </c>
+      <c r="S32" s="4">
+        <v>48</v>
+      </c>
+      <c r="T32" s="4">
+        <v>3</v>
+      </c>
+      <c r="U32" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2678,7 +2820,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -3345,16 +3487,16 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="3" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="C12" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3">
-        <v>275</v>
+        <v>230</v>
       </c>
       <c r="E12" s="4">
         <v>0</v>
@@ -3363,22 +3505,22 @@
         <v>0</v>
       </c>
       <c r="G12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="4">
         <v>0</v>
       </c>
       <c r="L12" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M12" s="4">
         <v>0</v>
@@ -3393,10 +3535,10 @@
         <v>3</v>
       </c>
       <c r="Q12" s="4">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="R12" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S12" s="4">
         <v>0</v>
@@ -3404,16 +3546,16 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="3" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13" s="3">
-        <v>218</v>
+        <v>275</v>
       </c>
       <c r="E13" s="4">
         <v>0</v>
@@ -3422,13 +3564,13 @@
         <v>0</v>
       </c>
       <c r="G13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="4">
         <v>0</v>
@@ -3437,10 +3579,10 @@
         <v>0</v>
       </c>
       <c r="L13" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M13" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N13" s="4">
         <v>0</v>
@@ -3452,10 +3594,10 @@
         <v>3</v>
       </c>
       <c r="Q13" s="4">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="R13" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="S13" s="4">
         <v>0</v>
@@ -3463,58 +3605,58 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" s="3">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3">
+        <v>218</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
+        <v>5</v>
+      </c>
+      <c r="M14" s="4">
+        <v>2</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0</v>
+      </c>
+      <c r="P14" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>0</v>
+      </c>
+      <c r="R14" s="4">
         <v>6</v>
-      </c>
-      <c r="D14" s="3">
-        <v>275</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0</v>
-      </c>
-      <c r="F14" s="4">
-        <v>0</v>
-      </c>
-      <c r="G14" s="4">
-        <v>1</v>
-      </c>
-      <c r="H14" s="4">
-        <v>0</v>
-      </c>
-      <c r="I14" s="4">
-        <v>3</v>
-      </c>
-      <c r="J14" s="4">
-        <v>0</v>
-      </c>
-      <c r="K14" s="4">
-        <v>0</v>
-      </c>
-      <c r="L14" s="4">
-        <v>4</v>
-      </c>
-      <c r="M14" s="4">
-        <v>2</v>
-      </c>
-      <c r="N14" s="4">
-        <v>1</v>
-      </c>
-      <c r="O14" s="4">
-        <v>0</v>
-      </c>
-      <c r="P14" s="4">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="4">
-        <v>0</v>
-      </c>
-      <c r="R14" s="4">
-        <v>3</v>
       </c>
       <c r="S14" s="4">
         <v>0</v>
@@ -3522,16 +3664,16 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" s="3">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E15" s="4">
         <v>0</v>
@@ -3540,37 +3682,37 @@
         <v>0</v>
       </c>
       <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>3</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
         <v>4</v>
       </c>
-      <c r="H15" s="4">
-        <v>0</v>
-      </c>
-      <c r="I15" s="4">
-        <v>1</v>
-      </c>
-      <c r="J15" s="4">
-        <v>0</v>
-      </c>
-      <c r="K15" s="4">
-        <v>0</v>
-      </c>
-      <c r="L15" s="4">
-        <v>1</v>
-      </c>
       <c r="M15" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15" s="4">
         <v>0</v>
       </c>
       <c r="P15" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="R15" s="4">
         <v>3</v>
@@ -3581,16 +3723,16 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="C16" s="3">
         <v>5</v>
       </c>
       <c r="D16" s="3">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="E16" s="4">
         <v>0</v>
@@ -3599,13 +3741,13 @@
         <v>0</v>
       </c>
       <c r="G16" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H16" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J16" s="4">
         <v>0</v>
@@ -3617,7 +3759,7 @@
         <v>1</v>
       </c>
       <c r="M16" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16" s="4">
         <v>0</v>
@@ -3626,13 +3768,13 @@
         <v>0</v>
       </c>
       <c r="P16" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="4">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="R16" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S16" s="4">
         <v>0</v>
@@ -3640,16 +3782,16 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C17" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D17" s="3">
-        <v>50</v>
+        <v>212</v>
       </c>
       <c r="E17" s="4">
         <v>0</v>
@@ -3658,13 +3800,13 @@
         <v>0</v>
       </c>
       <c r="G17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J17" s="4">
         <v>0</v>
@@ -3673,10 +3815,10 @@
         <v>0</v>
       </c>
       <c r="L17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" s="4">
         <v>0</v>
@@ -3685,10 +3827,10 @@
         <v>0</v>
       </c>
       <c r="P17" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q17" s="4">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="R17" s="4">
         <v>0</v>
@@ -3699,16 +3841,16 @@
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="3" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C18" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D18" s="3">
-        <v>297</v>
+        <v>50</v>
       </c>
       <c r="E18" s="4">
         <v>0</v>
@@ -3720,10 +3862,10 @@
         <v>0</v>
       </c>
       <c r="H18" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J18" s="4">
         <v>0</v>
@@ -3732,25 +3874,25 @@
         <v>0</v>
       </c>
       <c r="L18" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M18" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O18" s="4">
         <v>0</v>
       </c>
       <c r="P18" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="4">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="R18" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S18" s="4">
         <v>0</v>
@@ -3758,58 +3900,58 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="3">
+        <v>6</v>
+      </c>
+      <c r="D19" s="3">
+        <v>297</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1</v>
+      </c>
+      <c r="I19" s="4">
+        <v>4</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0</v>
+      </c>
+      <c r="L19" s="4">
+        <v>2</v>
+      </c>
+      <c r="M19" s="4">
+        <v>1</v>
+      </c>
+      <c r="N19" s="4">
+        <v>1</v>
+      </c>
+      <c r="O19" s="4">
+        <v>0</v>
+      </c>
+      <c r="P19" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="4">
         <v>35</v>
       </c>
-      <c r="C19" s="3">
-        <v>3</v>
-      </c>
-      <c r="D19" s="3">
-        <v>178</v>
-      </c>
-      <c r="E19" s="4">
-        <v>0</v>
-      </c>
-      <c r="F19" s="4">
-        <v>0</v>
-      </c>
-      <c r="G19" s="4">
-        <v>0</v>
-      </c>
-      <c r="H19" s="4">
-        <v>0</v>
-      </c>
-      <c r="I19" s="4">
-        <v>3</v>
-      </c>
-      <c r="J19" s="4">
-        <v>1</v>
-      </c>
-      <c r="K19" s="4">
-        <v>0</v>
-      </c>
-      <c r="L19" s="4">
-        <v>0</v>
-      </c>
-      <c r="M19" s="4">
-        <v>0</v>
-      </c>
-      <c r="N19" s="4">
-        <v>0</v>
-      </c>
-      <c r="O19" s="4">
-        <v>0</v>
-      </c>
-      <c r="P19" s="4">
-        <v>3</v>
-      </c>
-      <c r="Q19" s="4">
-        <v>45</v>
-      </c>
       <c r="R19" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S19" s="4">
         <v>0</v>
@@ -3817,22 +3959,22 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="3" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C20" s="3">
         <v>3</v>
       </c>
       <c r="D20" s="3">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="E20" s="4">
         <v>0</v>
       </c>
       <c r="F20" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" s="4">
         <v>0</v>
@@ -3841,34 +3983,34 @@
         <v>0</v>
       </c>
       <c r="I20" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="4">
         <v>0</v>
       </c>
       <c r="L20" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N20" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O20" s="4">
         <v>0</v>
       </c>
       <c r="P20" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q20" s="4">
+        <v>45</v>
+      </c>
+      <c r="R20" s="4">
         <v>5</v>
-      </c>
-      <c r="R20" s="4">
-        <v>6</v>
       </c>
       <c r="S20" s="4">
         <v>0</v>
@@ -3876,28 +4018,28 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" s="3" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C21" s="3">
         <v>3</v>
       </c>
       <c r="D21" s="3">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E21" s="4">
         <v>0</v>
       </c>
       <c r="F21" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" s="4">
         <v>2</v>
@@ -3912,10 +4054,10 @@
         <v>1</v>
       </c>
       <c r="M21" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O21" s="4">
         <v>0</v>
@@ -3924,10 +4066,10 @@
         <v>1</v>
       </c>
       <c r="Q21" s="4">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R21" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S21" s="4">
         <v>0</v>
@@ -3935,16 +4077,16 @@
     </row>
     <row r="22" spans="1:19">
       <c r="A22" s="3" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="C22" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D22" s="3">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="E22" s="4">
         <v>0</v>
@@ -3953,13 +4095,13 @@
         <v>0</v>
       </c>
       <c r="G22" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J22" s="4">
         <v>0</v>
@@ -3971,7 +4113,7 @@
         <v>1</v>
       </c>
       <c r="M22" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22" s="4">
         <v>0</v>
@@ -3980,13 +4122,13 @@
         <v>0</v>
       </c>
       <c r="P22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q22" s="4">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="R22" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S22" s="4">
         <v>0</v>
@@ -3994,43 +4136,43 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" s="3" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C23" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="3">
-        <v>244</v>
+        <v>139</v>
       </c>
       <c r="E23" s="4">
         <v>0</v>
       </c>
       <c r="F23" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23" s="4">
         <v>0</v>
       </c>
       <c r="I23" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J23" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" s="4">
         <v>0</v>
       </c>
       <c r="L23" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23" s="4">
         <v>0</v>
@@ -4039,13 +4181,13 @@
         <v>0</v>
       </c>
       <c r="P23" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="4">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="R23" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S23" s="4">
         <v>0</v>
@@ -4053,40 +4195,40 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C24" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" s="3">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E24" s="4">
         <v>0</v>
       </c>
       <c r="F24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I24" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="4">
         <v>0</v>
       </c>
       <c r="L24" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M24" s="4">
         <v>0</v>
@@ -4098,13 +4240,13 @@
         <v>0</v>
       </c>
       <c r="P24" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q24" s="4">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="R24" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S24" s="4">
         <v>0</v>
@@ -4112,16 +4254,16 @@
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="3" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="C25" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D25" s="3">
-        <v>52</v>
+        <v>242</v>
       </c>
       <c r="E25" s="4">
         <v>0</v>
@@ -4133,7 +4275,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I25" s="4">
         <v>1</v>
@@ -4145,7 +4287,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M25" s="4">
         <v>0</v>
@@ -4157,13 +4299,13 @@
         <v>0</v>
       </c>
       <c r="P25" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q25" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R25" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S25" s="4">
         <v>0</v>
@@ -4171,16 +4313,16 @@
     </row>
     <row r="26" spans="1:19">
       <c r="A26" s="3" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="C26" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D26" s="3">
-        <v>302</v>
+        <v>144</v>
       </c>
       <c r="E26" s="4">
         <v>0</v>
@@ -4189,13 +4331,13 @@
         <v>0</v>
       </c>
       <c r="G26" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H26" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I26" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J26" s="4">
         <v>0</v>
@@ -4216,30 +4358,30 @@
         <v>0</v>
       </c>
       <c r="P26" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="4">
-        <v>15</v>
+        <v>-3</v>
       </c>
       <c r="R26" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S26" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:19">
       <c r="A27" s="3" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C27" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D27" s="3">
-        <v>250</v>
+        <v>87</v>
       </c>
       <c r="E27" s="4">
         <v>0</v>
@@ -4248,10 +4390,10 @@
         <v>0</v>
       </c>
       <c r="G27" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H27" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" s="4">
         <v>1</v>
@@ -4263,10 +4405,10 @@
         <v>0</v>
       </c>
       <c r="L27" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M27" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N27" s="4">
         <v>0</v>
@@ -4275,30 +4417,30 @@
         <v>0</v>
       </c>
       <c r="P27" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q27" s="4">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="R27" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:19">
       <c r="A28" s="3" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C28" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D28" s="3">
-        <v>216</v>
+        <v>302</v>
       </c>
       <c r="E28" s="4">
         <v>0</v>
@@ -4307,13 +4449,13 @@
         <v>0</v>
       </c>
       <c r="G28" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H28" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I28" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J28" s="4">
         <v>0</v>
@@ -4334,30 +4476,30 @@
         <v>0</v>
       </c>
       <c r="P28" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q28" s="4">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="R28" s="4">
         <v>1</v>
       </c>
       <c r="S28" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:19">
       <c r="A29" s="3" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="C29" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D29" s="3">
-        <v>125</v>
+        <v>250</v>
       </c>
       <c r="E29" s="4">
         <v>0</v>
@@ -4366,22 +4508,22 @@
         <v>0</v>
       </c>
       <c r="G29" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H29" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J29" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29" s="4">
         <v>0</v>
       </c>
       <c r="L29" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M29" s="4">
         <v>1</v>
@@ -4393,13 +4535,13 @@
         <v>0</v>
       </c>
       <c r="P29" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q29" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R29" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S29" s="4">
         <v>0</v>
@@ -4407,60 +4549,178 @@
     </row>
     <row r="30" spans="1:19">
       <c r="A30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="3">
+        <v>5</v>
+      </c>
+      <c r="D30" s="3">
+        <v>216</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4">
+        <v>3</v>
+      </c>
+      <c r="H30" s="4">
+        <v>1</v>
+      </c>
+      <c r="I30" s="4">
+        <v>2</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0</v>
+      </c>
+      <c r="K30" s="4">
+        <v>0</v>
+      </c>
+      <c r="L30" s="4">
+        <v>2</v>
+      </c>
+      <c r="M30" s="4">
+        <v>0</v>
+      </c>
+      <c r="N30" s="4">
+        <v>0</v>
+      </c>
+      <c r="O30" s="4">
+        <v>0</v>
+      </c>
+      <c r="P30" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>7</v>
+      </c>
+      <c r="R30" s="4">
+        <v>1</v>
+      </c>
+      <c r="S30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="3">
+        <v>3</v>
+      </c>
+      <c r="D31" s="3">
+        <v>171</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0</v>
+      </c>
+      <c r="I31" s="4">
+        <v>2</v>
+      </c>
+      <c r="J31" s="4">
+        <v>1</v>
+      </c>
+      <c r="K31" s="4">
+        <v>0</v>
+      </c>
+      <c r="L31" s="4">
+        <v>1</v>
+      </c>
+      <c r="M31" s="4">
+        <v>1</v>
+      </c>
+      <c r="N31" s="4">
+        <v>0</v>
+      </c>
+      <c r="O31" s="4">
+        <v>0</v>
+      </c>
+      <c r="P31" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>11</v>
+      </c>
+      <c r="R31" s="4">
+        <v>5</v>
+      </c>
+      <c r="S31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C32" s="3">
         <v>4</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D32" s="3">
         <v>162</v>
       </c>
-      <c r="E30" s="4">
-        <v>0</v>
-      </c>
-      <c r="F30" s="4">
-        <v>0</v>
-      </c>
-      <c r="G30" s="4">
-        <v>2</v>
-      </c>
-      <c r="H30" s="4">
-        <v>1</v>
-      </c>
-      <c r="I30" s="4">
-        <v>1</v>
-      </c>
-      <c r="J30" s="4">
-        <v>0</v>
-      </c>
-      <c r="K30" s="4">
-        <v>0</v>
-      </c>
-      <c r="L30" s="4">
-        <v>2</v>
-      </c>
-      <c r="M30" s="4">
-        <v>1</v>
-      </c>
-      <c r="N30" s="4">
-        <v>0</v>
-      </c>
-      <c r="O30" s="4">
-        <v>0</v>
-      </c>
-      <c r="P30" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="4">
-        <v>0</v>
-      </c>
-      <c r="R30" s="4">
-        <v>2</v>
-      </c>
-      <c r="S30" s="4">
+      <c r="E32" s="4">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>2</v>
+      </c>
+      <c r="H32" s="4">
+        <v>1</v>
+      </c>
+      <c r="I32" s="4">
+        <v>1</v>
+      </c>
+      <c r="J32" s="4">
+        <v>0</v>
+      </c>
+      <c r="K32" s="4">
+        <v>0</v>
+      </c>
+      <c r="L32" s="4">
+        <v>2</v>
+      </c>
+      <c r="M32" s="4">
+        <v>1</v>
+      </c>
+      <c r="N32" s="4">
+        <v>0</v>
+      </c>
+      <c r="O32" s="4">
+        <v>0</v>
+      </c>
+      <c r="P32" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>0</v>
+      </c>
+      <c r="R32" s="4">
+        <v>2</v>
+      </c>
+      <c r="S32" s="4">
         <v>0</v>
       </c>
     </row>
@@ -4471,7 +4731,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -4744,10 +5004,10 @@
         <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -4756,25 +5016,25 @@
         <v>0</v>
       </c>
       <c r="G5" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H5" s="5">
         <v>0</v>
       </c>
       <c r="I5" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="K5" s="5">
         <v>0</v>
       </c>
       <c r="L5" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M5" s="5">
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="N5" s="5">
         <v>0</v>
@@ -4783,19 +5043,19 @@
         <v>0</v>
       </c>
       <c r="P5" s="5">
-        <v>1.75</v>
+        <v>-1.025</v>
       </c>
       <c r="Q5" s="5">
-        <v>0.4</v>
+        <v>-0.1</v>
       </c>
       <c r="R5" s="5">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="S5" s="5">
         <v>-0</v>
       </c>
       <c r="T5" s="5">
-        <v>6.850000000000001</v>
+        <v>6.625</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -4806,10 +5066,10 @@
         <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
@@ -4818,25 +5078,25 @@
         <v>0</v>
       </c>
       <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>3</v>
+      </c>
+      <c r="J6" s="5">
         <v>0.75</v>
       </c>
-      <c r="H6" s="5">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>1</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0</v>
-      </c>
       <c r="K6" s="5">
         <v>0</v>
       </c>
       <c r="L6" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M6" s="5">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="N6" s="5">
         <v>0</v>
@@ -4845,10 +5105,10 @@
         <v>0</v>
       </c>
       <c r="P6" s="5">
-        <v>-1.025</v>
+        <v>1.433333333333334</v>
       </c>
       <c r="Q6" s="5">
-        <v>-0.1</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="R6" s="5">
         <v>0.5</v>
@@ -4857,7 +5117,7 @@
         <v>-0</v>
       </c>
       <c r="T6" s="5">
-        <v>6.625</v>
+        <v>6.283333333333333</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -4868,10 +5128,10 @@
         <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
@@ -4883,22 +5143,22 @@
         <v>0</v>
       </c>
       <c r="H7" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I7" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J7" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="K7" s="5">
         <v>0</v>
       </c>
       <c r="L7" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M7" s="5">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N7" s="5">
         <v>0</v>
@@ -4907,19 +5167,19 @@
         <v>0</v>
       </c>
       <c r="P7" s="5">
-        <v>1.433333333333334</v>
+        <v>-0.1399999999999999</v>
       </c>
       <c r="Q7" s="5">
+        <v>-0.9</v>
+      </c>
+      <c r="R7" s="5">
         <v>0.6000000000000001</v>
-      </c>
-      <c r="R7" s="5">
-        <v>0.5</v>
       </c>
       <c r="S7" s="5">
         <v>-0</v>
       </c>
       <c r="T7" s="5">
-        <v>6.283333333333333</v>
+        <v>6.210000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -4930,13 +5190,13 @@
         <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="E8" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F8" s="5">
         <v>0</v>
@@ -4945,22 +5205,22 @@
         <v>0</v>
       </c>
       <c r="H8" s="5">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I8" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J8" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K8" s="5">
         <v>0</v>
       </c>
       <c r="L8" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M8" s="5">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="N8" s="5">
         <v>0</v>
@@ -4969,19 +5229,19 @@
         <v>0</v>
       </c>
       <c r="P8" s="5">
-        <v>-0.1399999999999999</v>
+        <v>0.3399999999999999</v>
       </c>
       <c r="Q8" s="5">
-        <v>-0.9</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="R8" s="5">
-        <v>0.6000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="S8" s="5">
         <v>-0</v>
       </c>
       <c r="T8" s="5">
-        <v>6.210000000000001</v>
+        <v>6.206666666666667</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -4992,13 +5252,13 @@
         <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="E9" s="5">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F9" s="5">
         <v>0</v>
@@ -5007,10 +5267,10 @@
         <v>0</v>
       </c>
       <c r="H9" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I9" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9" s="5">
         <v>0.75</v>
@@ -5019,10 +5279,10 @@
         <v>0</v>
       </c>
       <c r="L9" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M9" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="N9" s="5">
         <v>0</v>
@@ -5031,19 +5291,19 @@
         <v>0</v>
       </c>
       <c r="P9" s="5">
-        <v>0.3399999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="Q9" s="5">
-        <v>0.1666666666666666</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="R9" s="5">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="S9" s="5">
         <v>-0</v>
       </c>
       <c r="T9" s="5">
-        <v>6.206666666666667</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -5054,16 +5314,16 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
       </c>
       <c r="F10" s="5">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G10" s="5">
         <v>0</v>
@@ -5075,7 +5335,7 @@
         <v>2</v>
       </c>
       <c r="J10" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K10" s="5">
         <v>0</v>
@@ -5087,25 +5347,25 @@
         <v>0.75</v>
       </c>
       <c r="N10" s="5">
+        <v>0</v>
+      </c>
+      <c r="O10" s="5">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>-0.35</v>
+      </c>
+      <c r="R10" s="5">
         <v>0.5</v>
-      </c>
-      <c r="O10" s="5">
-        <v>0</v>
-      </c>
-      <c r="P10" s="5">
-        <v>0.7666666666666665</v>
-      </c>
-      <c r="Q10" s="5">
-        <v>-0.4</v>
-      </c>
-      <c r="R10" s="5">
-        <v>0.6000000000000001</v>
       </c>
       <c r="S10" s="5">
         <v>-0</v>
       </c>
       <c r="T10" s="5">
-        <v>5.616666666666667</v>
+        <v>5.850000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -5116,25 +5376,25 @@
         <v>25</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="E11" s="5">
         <v>0</v>
       </c>
       <c r="F11" s="5">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="5">
         <v>0</v>
       </c>
       <c r="I11" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" s="5">
         <v>0</v>
@@ -5143,22 +5403,22 @@
         <v>0</v>
       </c>
       <c r="L11" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M11" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N11" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O11" s="5">
         <v>0</v>
       </c>
       <c r="P11" s="5">
-        <v>-0.1333333333333336</v>
+        <v>0.7666666666666665</v>
       </c>
       <c r="Q11" s="5">
-        <v>-0.1</v>
+        <v>-0.4</v>
       </c>
       <c r="R11" s="5">
         <v>0.6000000000000001</v>
@@ -5167,7 +5427,7 @@
         <v>-0</v>
       </c>
       <c r="T11" s="5">
-        <v>5.366666666666667</v>
+        <v>5.616666666666667</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -5178,10 +5438,10 @@
         <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
@@ -5190,13 +5450,13 @@
         <v>0</v>
       </c>
       <c r="G12" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="5">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="I12" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J12" s="5">
         <v>0</v>
@@ -5205,7 +5465,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M12" s="5">
         <v>0</v>
@@ -5217,19 +5477,19 @@
         <v>0</v>
       </c>
       <c r="P12" s="5">
-        <v>0.5333333333333335</v>
+        <v>-0.1333333333333336</v>
       </c>
       <c r="Q12" s="5">
-        <v>-0.4</v>
+        <v>-0.1</v>
       </c>
       <c r="R12" s="5">
-        <v>0.1</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="S12" s="5">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="T12" s="5">
-        <v>4.683333333333333</v>
+        <v>5.366666666666667</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -5240,10 +5500,10 @@
         <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E13" s="5">
         <v>0</v>
@@ -5252,13 +5512,13 @@
         <v>0</v>
       </c>
       <c r="G13" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="H13" s="5">
-        <v>0.15</v>
+        <v>0.45</v>
       </c>
       <c r="I13" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J13" s="5">
         <v>0</v>
@@ -5279,19 +5539,19 @@
         <v>0</v>
       </c>
       <c r="P13" s="5">
-        <v>-0.1799999999999997</v>
+        <v>0.5333333333333335</v>
       </c>
       <c r="Q13" s="5">
-        <v>-0.2</v>
+        <v>-0.4</v>
       </c>
       <c r="R13" s="5">
         <v>0.1</v>
       </c>
       <c r="S13" s="5">
-        <v>-0</v>
+        <v>-1</v>
       </c>
       <c r="T13" s="5">
-        <v>4.62</v>
+        <v>4.683333333333333</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -5302,10 +5562,10 @@
         <v>25</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="E14" s="5">
         <v>0</v>
@@ -5314,7 +5574,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="5">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="H14" s="5">
         <v>0.15</v>
@@ -5329,7 +5589,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M14" s="5">
         <v>0</v>
@@ -5341,19 +5601,19 @@
         <v>0</v>
       </c>
       <c r="P14" s="5">
-        <v>0.6666666666666665</v>
+        <v>-0.1799999999999997</v>
       </c>
       <c r="Q14" s="5">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="R14" s="5">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="S14" s="5">
         <v>-0</v>
       </c>
       <c r="T14" s="5">
-        <v>4.566666666666666</v>
+        <v>4.62</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -5364,16 +5624,16 @@
         <v>25</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="E15" s="5">
         <v>0</v>
       </c>
       <c r="F15" s="5">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G15" s="5">
         <v>0.25</v>
@@ -5385,13 +5645,13 @@
         <v>2</v>
       </c>
       <c r="J15" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="K15" s="5">
         <v>0</v>
       </c>
       <c r="L15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" s="5">
         <v>0</v>
@@ -5403,19 +5663,19 @@
         <v>0</v>
       </c>
       <c r="P15" s="5">
-        <v>0.175</v>
+        <v>0.6666666666666665</v>
       </c>
       <c r="Q15" s="5">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="R15" s="5">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="S15" s="5">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="T15" s="5">
-        <v>4.325</v>
+        <v>4.566666666666666</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -5426,37 +5686,37 @@
         <v>25</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E16" s="5">
         <v>0</v>
       </c>
       <c r="F16" s="5">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G16" s="5">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="H16" s="5">
         <v>0.15</v>
       </c>
       <c r="I16" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J16" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K16" s="5">
         <v>0</v>
       </c>
       <c r="L16" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M16" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="N16" s="5">
         <v>0</v>
@@ -5465,19 +5725,19 @@
         <v>0</v>
       </c>
       <c r="P16" s="5">
-        <v>-0.45</v>
+        <v>0.175</v>
       </c>
       <c r="Q16" s="5">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="R16" s="5">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="S16" s="5">
-        <v>-0</v>
+        <v>-1</v>
       </c>
       <c r="T16" s="5">
-        <v>4.15</v>
+        <v>4.325</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -5488,10 +5748,10 @@
         <v>25</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
@@ -5527,19 +5787,19 @@
         <v>0</v>
       </c>
       <c r="P17" s="5">
-        <v>-0.3333333333333336</v>
+        <v>-0.45</v>
       </c>
       <c r="Q17" s="5">
-        <v>-0.4333333333333333</v>
+        <v>0</v>
       </c>
       <c r="R17" s="5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="S17" s="5">
         <v>-0</v>
       </c>
       <c r="T17" s="5">
-        <v>4.033333333333333</v>
+        <v>4.15</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -5550,10 +5810,10 @@
         <v>25</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E18" s="5">
         <v>0</v>
@@ -5562,13 +5822,13 @@
         <v>0</v>
       </c>
       <c r="G18" s="5">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H18" s="5">
         <v>0.15</v>
       </c>
       <c r="I18" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J18" s="5">
         <v>0</v>
@@ -5577,7 +5837,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M18" s="5">
         <v>0.75</v>
@@ -5589,19 +5849,19 @@
         <v>0</v>
       </c>
       <c r="P18" s="5">
-        <v>-0.2600000000000002</v>
+        <v>-0.3333333333333336</v>
       </c>
       <c r="Q18" s="5">
-        <v>-0.1333333333333333</v>
+        <v>-0.4333333333333333</v>
       </c>
       <c r="R18" s="5">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="S18" s="5">
         <v>-0</v>
       </c>
       <c r="T18" s="5">
-        <v>3.756666666666667</v>
+        <v>4.033333333333333</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -5612,16 +5872,16 @@
         <v>25</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="E19" s="5">
         <v>0</v>
       </c>
       <c r="F19" s="5">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G19" s="5">
         <v>0.25</v>
@@ -5630,7 +5890,7 @@
         <v>0.15</v>
       </c>
       <c r="I19" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J19" s="5">
         <v>0</v>
@@ -5639,10 +5899,10 @@
         <v>0</v>
       </c>
       <c r="L19" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M19" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N19" s="5">
         <v>0</v>
@@ -5651,19 +5911,19 @@
         <v>0</v>
       </c>
       <c r="P19" s="5">
-        <v>0.2</v>
+        <v>-0.2600000000000002</v>
       </c>
       <c r="Q19" s="5">
-        <v>-0.4</v>
+        <v>-0.1333333333333333</v>
       </c>
       <c r="R19" s="5">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="S19" s="5">
-        <v>-0.5</v>
+        <v>-0</v>
       </c>
       <c r="T19" s="5">
-        <v>3.5</v>
+        <v>3.756666666666667</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -5674,10 +5934,10 @@
         <v>25</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="E20" s="5">
         <v>0</v>
@@ -5686,13 +5946,13 @@
         <v>0.4</v>
       </c>
       <c r="G20" s="5">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="H20" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I20" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J20" s="5">
         <v>0</v>
@@ -5701,7 +5961,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M20" s="5">
         <v>0</v>
@@ -5713,19 +5973,19 @@
         <v>0</v>
       </c>
       <c r="P20" s="5">
-        <v>-0.2166666666666665</v>
+        <v>0.2</v>
       </c>
       <c r="Q20" s="5">
-        <v>0</v>
+        <v>-0.4</v>
       </c>
       <c r="R20" s="5">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="S20" s="5">
         <v>-0.5</v>
       </c>
       <c r="T20" s="5">
-        <v>3.483333333333333</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -5736,10 +5996,10 @@
         <v>25</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="E21" s="5">
         <v>0</v>
@@ -5748,13 +6008,13 @@
         <v>0</v>
       </c>
       <c r="G21" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H21" s="5">
         <v>0</v>
       </c>
       <c r="I21" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J21" s="5">
         <v>0</v>
@@ -5763,7 +6023,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M21" s="5">
         <v>0</v>
@@ -5775,19 +6035,19 @@
         <v>0</v>
       </c>
       <c r="P21" s="5">
-        <v>-0.1200000000000003</v>
+        <v>0.3</v>
       </c>
       <c r="Q21" s="5">
-        <v>-0.2</v>
+        <v>-1.2</v>
       </c>
       <c r="R21" s="5">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="S21" s="5">
-        <v>-0</v>
+        <v>-0.5</v>
       </c>
       <c r="T21" s="5">
-        <v>2.98</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -5798,58 +6058,58 @@
         <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E22" s="5">
         <v>0</v>
       </c>
       <c r="F22" s="5">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G22" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
+        <v>2</v>
+      </c>
+      <c r="J22" s="5">
+        <v>0</v>
+      </c>
+      <c r="K22" s="5">
+        <v>0</v>
+      </c>
+      <c r="L22" s="5">
+        <v>1</v>
+      </c>
+      <c r="M22" s="5">
+        <v>0</v>
+      </c>
+      <c r="N22" s="5">
+        <v>0</v>
+      </c>
+      <c r="O22" s="5">
+        <v>0</v>
+      </c>
+      <c r="P22" s="5">
+        <v>-0.2166666666666665</v>
+      </c>
+      <c r="Q22" s="5">
+        <v>0</v>
+      </c>
+      <c r="R22" s="5">
         <v>0.3</v>
       </c>
-      <c r="I22" s="5">
-        <v>1</v>
-      </c>
-      <c r="J22" s="5">
-        <v>0</v>
-      </c>
-      <c r="K22" s="5">
-        <v>0</v>
-      </c>
-      <c r="L22" s="5">
-        <v>2</v>
-      </c>
-      <c r="M22" s="5">
-        <v>0</v>
-      </c>
-      <c r="N22" s="5">
-        <v>0</v>
-      </c>
-      <c r="O22" s="5">
-        <v>0</v>
-      </c>
-      <c r="P22" s="5">
-        <v>-0.4666666666666665</v>
-      </c>
-      <c r="Q22" s="5">
-        <v>-0.65</v>
-      </c>
-      <c r="R22" s="5">
-        <v>0.5</v>
-      </c>
       <c r="S22" s="5">
-        <v>-0</v>
+        <v>-0.5</v>
       </c>
       <c r="T22" s="5">
-        <v>2.683333333333334</v>
+        <v>3.483333333333333</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -5860,10 +6120,10 @@
         <v>25</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E23" s="5">
         <v>0</v>
@@ -5872,7 +6132,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="5">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H23" s="5">
         <v>0</v>
@@ -5890,28 +6150,28 @@
         <v>1</v>
       </c>
       <c r="M23" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="N23" s="5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O23" s="5">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="P23" s="5">
-        <v>-0.25</v>
+        <v>-0.1200000000000003</v>
       </c>
       <c r="Q23" s="5">
-        <v>-0.75</v>
+        <v>-0.2</v>
       </c>
       <c r="R23" s="5">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="S23" s="5">
-        <v>-0.5</v>
+        <v>-0</v>
       </c>
       <c r="T23" s="5">
-        <v>2.65</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="24" spans="1:20">
@@ -5922,10 +6182,10 @@
         <v>25</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="E24" s="5">
         <v>0</v>
@@ -5934,7 +6194,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="5">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="H24" s="5">
         <v>0.3</v>
@@ -5949,7 +6209,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M24" s="5">
         <v>0</v>
@@ -5961,19 +6221,19 @@
         <v>0</v>
       </c>
       <c r="P24" s="5">
-        <v>0.08333333333333358</v>
+        <v>-0.4666666666666665</v>
       </c>
       <c r="Q24" s="5">
-        <v>0.2333333333333334</v>
+        <v>-0.65</v>
       </c>
       <c r="R24" s="5">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="S24" s="5">
         <v>-0</v>
       </c>
       <c r="T24" s="5">
-        <v>2.066666666666667</v>
+        <v>2.683333333333334</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -5984,10 +6244,10 @@
         <v>25</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E25" s="5">
         <v>0</v>
@@ -5996,10 +6256,10 @@
         <v>0</v>
       </c>
       <c r="G25" s="5">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H25" s="5">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I25" s="5">
         <v>1</v>
@@ -6011,31 +6271,31 @@
         <v>0</v>
       </c>
       <c r="L25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N25" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O25" s="5">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="P25" s="5">
-        <v>0.1</v>
+        <v>-0.25</v>
       </c>
       <c r="Q25" s="5">
-        <v>0.7000000000000001</v>
+        <v>-0.75</v>
       </c>
       <c r="R25" s="5">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="S25" s="5">
         <v>-0.5</v>
       </c>
       <c r="T25" s="5">
-        <v>1.65</v>
+        <v>2.65</v>
       </c>
     </row>
     <row r="26" spans="1:20">
@@ -6046,10 +6306,10 @@
         <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E26" s="5">
         <v>0</v>
@@ -6058,13 +6318,13 @@
         <v>0</v>
       </c>
       <c r="G26" s="5">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="H26" s="5">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="5">
         <v>0</v>
@@ -6073,10 +6333,10 @@
         <v>0</v>
       </c>
       <c r="L26" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26" s="5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="N26" s="5">
         <v>0</v>
@@ -6085,10 +6345,10 @@
         <v>0</v>
       </c>
       <c r="P26" s="5">
-        <v>-1.025</v>
+        <v>0.08333333333333358</v>
       </c>
       <c r="Q26" s="5">
-        <v>0</v>
+        <v>0.2333333333333334</v>
       </c>
       <c r="R26" s="5">
         <v>0.2</v>
@@ -6097,7 +6357,7 @@
         <v>-0</v>
       </c>
       <c r="T26" s="5">
-        <v>1.425</v>
+        <v>2.066666666666667</v>
       </c>
     </row>
     <row r="27" spans="1:20">
@@ -6108,19 +6368,19 @@
         <v>25</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="E27" s="5">
         <v>0</v>
       </c>
       <c r="F27" s="5">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G27" s="5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H27" s="5">
         <v>0.15</v>
@@ -6147,19 +6407,19 @@
         <v>0</v>
       </c>
       <c r="P27" s="5">
-        <v>-0.01666666666666643</v>
+        <v>0.1</v>
       </c>
       <c r="Q27" s="5">
-        <v>-0.9</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="R27" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="S27" s="5">
-        <v>-0</v>
+        <v>-0.5</v>
       </c>
       <c r="T27" s="5">
-        <v>1.233333333333333</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="28" spans="1:20">
@@ -6170,10 +6430,10 @@
         <v>25</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="E28" s="5">
         <v>0</v>
@@ -6182,13 +6442,13 @@
         <v>0</v>
       </c>
       <c r="G28" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H28" s="5">
         <v>0</v>
       </c>
       <c r="I28" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" s="5">
         <v>0</v>
@@ -6197,10 +6457,10 @@
         <v>0</v>
       </c>
       <c r="L28" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28" s="5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="N28" s="5">
         <v>0</v>
@@ -6209,10 +6469,10 @@
         <v>0</v>
       </c>
       <c r="P28" s="5">
-        <v>0.7000000000000001</v>
+        <v>-1.025</v>
       </c>
       <c r="Q28" s="5">
-        <v>-0.9</v>
+        <v>0</v>
       </c>
       <c r="R28" s="5">
         <v>0.2</v>
@@ -6221,7 +6481,7 @@
         <v>-0</v>
       </c>
       <c r="T28" s="5">
-        <v>1</v>
+        <v>1.425</v>
       </c>
     </row>
     <row r="29" spans="1:20">
@@ -6232,22 +6492,22 @@
         <v>25</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="E29" s="5">
         <v>0</v>
       </c>
       <c r="F29" s="5">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G29" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H29" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I29" s="5">
         <v>1</v>
@@ -6271,19 +6531,19 @@
         <v>0</v>
       </c>
       <c r="P29" s="5">
-        <v>0.5</v>
+        <v>-0.01666666666666643</v>
       </c>
       <c r="Q29" s="5">
         <v>-0.9</v>
       </c>
       <c r="R29" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="S29" s="5">
         <v>-0</v>
       </c>
       <c r="T29" s="5">
-        <v>0.6</v>
+        <v>1.233333333333333</v>
       </c>
     </row>
     <row r="30" spans="1:20">
@@ -6294,10 +6554,10 @@
         <v>25</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="E30" s="5">
         <v>0</v>
@@ -6312,7 +6572,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="5">
         <v>0</v>
@@ -6333,18 +6593,142 @@
         <v>0</v>
       </c>
       <c r="P30" s="5">
+        <v>-0.15</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>-0.9</v>
+      </c>
+      <c r="R30" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="S30" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="T30" s="5">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0</v>
+      </c>
+      <c r="I31" s="5">
+        <v>1</v>
+      </c>
+      <c r="J31" s="5">
+        <v>0</v>
+      </c>
+      <c r="K31" s="5">
+        <v>0</v>
+      </c>
+      <c r="L31" s="5">
+        <v>0</v>
+      </c>
+      <c r="M31" s="5">
+        <v>0</v>
+      </c>
+      <c r="N31" s="5">
+        <v>0</v>
+      </c>
+      <c r="O31" s="5">
+        <v>0</v>
+      </c>
+      <c r="P31" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="Q31" s="5">
+        <v>-0.9</v>
+      </c>
+      <c r="R31" s="5">
+        <v>0</v>
+      </c>
+      <c r="S31" s="5">
+        <v>-0</v>
+      </c>
+      <c r="T31" s="5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0</v>
+      </c>
+      <c r="F32" s="5">
+        <v>0</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5">
+        <v>0</v>
+      </c>
+      <c r="J32" s="5">
+        <v>0</v>
+      </c>
+      <c r="K32" s="5">
+        <v>0</v>
+      </c>
+      <c r="L32" s="5">
+        <v>1</v>
+      </c>
+      <c r="M32" s="5">
+        <v>0</v>
+      </c>
+      <c r="N32" s="5">
+        <v>0</v>
+      </c>
+      <c r="O32" s="5">
+        <v>0</v>
+      </c>
+      <c r="P32" s="5">
         <v>-0.425</v>
       </c>
-      <c r="Q30" s="5">
+      <c r="Q32" s="5">
         <v>-0.6666666666666666</v>
       </c>
-      <c r="R30" s="5">
+      <c r="R32" s="5">
         <v>0.1</v>
       </c>
-      <c r="S30" s="5">
+      <c r="S32" s="5">
         <v>-0</v>
       </c>
-      <c r="T30" s="5">
+      <c r="T32" s="5">
         <v>0.2583333333333333</v>
       </c>
     </row>

</xml_diff>